<commit_message>
getter functions and landscape objects
</commit_message>
<xml_diff>
--- a/config/kingdom_regular.xlsx
+++ b/config/kingdom_regular.xlsx
@@ -1972,7 +1972,7 @@
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>GUILDS</t>
+          <t>HINTERLANDS</t>
         </is>
       </c>
       <c r="B94" s="1" t="inlineStr">
@@ -1991,24 +1991,20 @@
         </is>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n"/>
       <c r="B95" s="1" t="n"/>
-      <c r="C95" s="1" t="inlineStr">
-        <is>
-          <t>FOUR</t>
-        </is>
-      </c>
+      <c r="C95" s="1" t="n"/>
       <c r="D95" s="1" t="inlineStr">
         <is>
-          <t>ACTION</t>
+          <t>TREASURE</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -2016,16 +2012,12 @@
       <c r="B96" s="1" t="n"/>
       <c r="C96" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
-        </is>
-      </c>
-      <c r="D96" s="1" t="inlineStr">
-        <is>
-          <t>ACTION</t>
-        </is>
-      </c>
+          <t>THREE</t>
+        </is>
+      </c>
+      <c r="D96" s="1" t="inlineStr"/>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -2034,23 +2026,19 @@
       <c r="C97" s="1" t="n"/>
       <c r="D97" s="1" t="inlineStr">
         <is>
-          <t>ACTION - ATTACK</t>
+          <t>ACTION</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n"/>
-      <c r="B98" s="1" t="inlineStr">
-        <is>
-          <t>1RC</t>
-        </is>
-      </c>
+      <c r="B98" s="1" t="n"/>
       <c r="C98" s="1" t="inlineStr">
         <is>
-          <t>THREE</t>
+          <t>FOUR</t>
         </is>
       </c>
       <c r="D98" s="1" t="inlineStr">
@@ -2059,30 +2047,30 @@
         </is>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n"/>
       <c r="B99" s="1" t="n"/>
-      <c r="C99" s="1" t="n"/>
+      <c r="C99" s="1" t="inlineStr">
+        <is>
+          <t>FIVE</t>
+        </is>
+      </c>
       <c r="D99" s="1" t="inlineStr">
         <is>
-          <t>TREASURE</t>
+          <t>ACTION</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n"/>
       <c r="B100" s="1" t="n"/>
-      <c r="C100" s="1" t="inlineStr">
-        <is>
-          <t>FOUR</t>
-        </is>
-      </c>
+      <c r="C100" s="1" t="n"/>
       <c r="D100" s="1" t="inlineStr">
         <is>
           <t>ACTION - ATTACK</t>
@@ -2093,26 +2081,14 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="1" t="inlineStr">
-        <is>
-          <t>CORNUCOPIA_GUILDS</t>
-        </is>
-      </c>
-      <c r="B101" s="1" t="inlineStr">
-        <is>
-          <t>2ND</t>
-        </is>
-      </c>
+      <c r="A101" s="1" t="n"/>
+      <c r="B101" s="1" t="n"/>
       <c r="C101" s="1" t="inlineStr">
         <is>
-          <t>TWO</t>
-        </is>
-      </c>
-      <c r="D101" s="1" t="inlineStr">
-        <is>
-          <t>ACTION</t>
-        </is>
-      </c>
+          <t>OTHER</t>
+        </is>
+      </c>
+      <c r="D101" s="1" t="inlineStr"/>
       <c r="E101" t="n">
         <v>1</v>
       </c>
@@ -2120,26 +2096,26 @@
     <row r="102">
       <c r="A102" s="1" t="n"/>
       <c r="B102" s="1" t="n"/>
-      <c r="C102" s="1" t="inlineStr">
-        <is>
-          <t>THREE</t>
-        </is>
-      </c>
+      <c r="C102" s="1" t="n"/>
       <c r="D102" s="1" t="inlineStr">
         <is>
           <t>ACTION</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n"/>
-      <c r="B103" s="1" t="n"/>
+      <c r="B103" s="1" t="inlineStr">
+        <is>
+          <t>2ND</t>
+        </is>
+      </c>
       <c r="C103" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
+          <t>THREE</t>
         </is>
       </c>
       <c r="D103" s="1" t="inlineStr">
@@ -2156,7 +2132,7 @@
       <c r="B104" s="1" t="n"/>
       <c r="C104" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>FOUR</t>
         </is>
       </c>
       <c r="D104" s="1" t="inlineStr">
@@ -2165,45 +2141,37 @@
         </is>
       </c>
       <c r="E104" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n"/>
       <c r="B105" s="1" t="n"/>
-      <c r="C105" s="1" t="n"/>
+      <c r="C105" s="1" t="inlineStr">
+        <is>
+          <t>FIVE</t>
+        </is>
+      </c>
       <c r="D105" s="1" t="inlineStr">
         <is>
+          <t>ACTION</t>
+        </is>
+      </c>
+      <c r="E105" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n"/>
+      <c r="B106" s="1" t="n"/>
+      <c r="C106" s="1" t="n"/>
+      <c r="D106" s="1" t="inlineStr">
+        <is>
           <t>ACTION - ATTACK</t>
         </is>
       </c>
-      <c r="E105" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="inlineStr">
-        <is>
-          <t>HINTERLANDS</t>
-        </is>
-      </c>
-      <c r="B106" s="1" t="inlineStr">
-        <is>
-          <t>1ST</t>
-        </is>
-      </c>
-      <c r="C106" s="1" t="inlineStr">
-        <is>
-          <t>TWO</t>
-        </is>
-      </c>
-      <c r="D106" s="1" t="inlineStr">
-        <is>
-          <t>ACTION</t>
-        </is>
-      </c>
       <c r="E106" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107">
@@ -2212,7 +2180,7 @@
       <c r="C107" s="1" t="n"/>
       <c r="D107" s="1" t="inlineStr">
         <is>
-          <t>TREASURE</t>
+          <t>ATTACK - TREASURE</t>
         </is>
       </c>
       <c r="E107" t="n">
@@ -2221,13 +2189,21 @@
     </row>
     <row r="108">
       <c r="A108" s="1" t="n"/>
-      <c r="B108" s="1" t="n"/>
+      <c r="B108" s="1" t="inlineStr">
+        <is>
+          <t>1RC</t>
+        </is>
+      </c>
       <c r="C108" s="1" t="inlineStr">
         <is>
-          <t>THREE</t>
-        </is>
-      </c>
-      <c r="D108" s="1" t="inlineStr"/>
+          <t>TWO</t>
+        </is>
+      </c>
+      <c r="D108" s="1" t="inlineStr">
+        <is>
+          <t>ACTION</t>
+        </is>
+      </c>
       <c r="E108" t="n">
         <v>1</v>
       </c>
@@ -2235,14 +2211,18 @@
     <row r="109">
       <c r="A109" s="1" t="n"/>
       <c r="B109" s="1" t="n"/>
-      <c r="C109" s="1" t="n"/>
+      <c r="C109" s="1" t="inlineStr">
+        <is>
+          <t>THREE</t>
+        </is>
+      </c>
       <c r="D109" s="1" t="inlineStr">
         <is>
-          <t>ACTION</t>
+          <t>ACTION - ATTACK</t>
         </is>
       </c>
       <c r="E109" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
@@ -2253,30 +2233,22 @@
           <t>FOUR</t>
         </is>
       </c>
-      <c r="D110" s="1" t="inlineStr">
-        <is>
-          <t>ACTION</t>
-        </is>
-      </c>
+      <c r="D110" s="1" t="inlineStr"/>
       <c r="E110" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n"/>
       <c r="B111" s="1" t="n"/>
-      <c r="C111" s="1" t="inlineStr">
-        <is>
-          <t>FIVE</t>
-        </is>
-      </c>
+      <c r="C111" s="1" t="n"/>
       <c r="D111" s="1" t="inlineStr">
         <is>
           <t>ACTION</t>
         </is>
       </c>
       <c r="E111" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -2297,12 +2269,16 @@
       <c r="B113" s="1" t="n"/>
       <c r="C113" s="1" t="inlineStr">
         <is>
-          <t>OTHER</t>
-        </is>
-      </c>
-      <c r="D113" s="1" t="inlineStr"/>
+          <t>FIVE</t>
+        </is>
+      </c>
+      <c r="D113" s="1" t="inlineStr">
+        <is>
+          <t>ACTION</t>
+        </is>
+      </c>
       <c r="E113" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114">
@@ -2311,23 +2287,27 @@
       <c r="C114" s="1" t="n"/>
       <c r="D114" s="1" t="inlineStr">
         <is>
-          <t>ACTION</t>
+          <t>TREASURE</t>
         </is>
       </c>
       <c r="E114" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="1" t="n"/>
+      <c r="A115" s="1" t="inlineStr">
+        <is>
+          <t>DARK_AGES</t>
+        </is>
+      </c>
       <c r="B115" s="1" t="inlineStr">
         <is>
-          <t>2ND</t>
+          <t>1ST</t>
         </is>
       </c>
       <c r="C115" s="1" t="inlineStr">
         <is>
-          <t>THREE</t>
+          <t>TWO</t>
         </is>
       </c>
       <c r="D115" s="1" t="inlineStr">
@@ -2336,7 +2316,7 @@
         </is>
       </c>
       <c r="E115" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116">
@@ -2344,7 +2324,7 @@
       <c r="B116" s="1" t="n"/>
       <c r="C116" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
+          <t>THREE</t>
         </is>
       </c>
       <c r="D116" s="1" t="inlineStr">
@@ -2353,37 +2333,33 @@
         </is>
       </c>
       <c r="E116" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n"/>
       <c r="B117" s="1" t="n"/>
-      <c r="C117" s="1" t="inlineStr">
-        <is>
-          <t>FIVE</t>
-        </is>
-      </c>
+      <c r="C117" s="1" t="n"/>
       <c r="D117" s="1" t="inlineStr">
         <is>
-          <t>ACTION</t>
+          <t>ACTION - ATTACK</t>
         </is>
       </c>
       <c r="E117" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n"/>
       <c r="B118" s="1" t="n"/>
-      <c r="C118" s="1" t="n"/>
-      <c r="D118" s="1" t="inlineStr">
-        <is>
-          <t>ACTION - ATTACK</t>
-        </is>
-      </c>
+      <c r="C118" s="1" t="inlineStr">
+        <is>
+          <t>FOUR</t>
+        </is>
+      </c>
+      <c r="D118" s="1" t="inlineStr"/>
       <c r="E118" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
@@ -2392,28 +2368,20 @@
       <c r="C119" s="1" t="n"/>
       <c r="D119" s="1" t="inlineStr">
         <is>
-          <t>ATTACK - TREASURE</t>
+          <t>ACTION</t>
         </is>
       </c>
       <c r="E119" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n"/>
-      <c r="B120" s="1" t="inlineStr">
-        <is>
-          <t>1RC</t>
-        </is>
-      </c>
-      <c r="C120" s="1" t="inlineStr">
-        <is>
-          <t>TWO</t>
-        </is>
-      </c>
+      <c r="B120" s="1" t="n"/>
+      <c r="C120" s="1" t="n"/>
       <c r="D120" s="1" t="inlineStr">
         <is>
-          <t>ACTION</t>
+          <t>ACTION - ATTACK - LOOTER</t>
         </is>
       </c>
       <c r="E120" t="n">
@@ -2423,14 +2391,10 @@
     <row r="121">
       <c r="A121" s="1" t="n"/>
       <c r="B121" s="1" t="n"/>
-      <c r="C121" s="1" t="inlineStr">
-        <is>
-          <t>THREE</t>
-        </is>
-      </c>
+      <c r="C121" s="1" t="n"/>
       <c r="D121" s="1" t="inlineStr">
         <is>
-          <t>ACTION - ATTACK</t>
+          <t>ACTION - LOOTER</t>
         </is>
       </c>
       <c r="E121" t="n">
@@ -2442,12 +2406,16 @@
       <c r="B122" s="1" t="n"/>
       <c r="C122" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
-        </is>
-      </c>
-      <c r="D122" s="1" t="inlineStr"/>
+          <t>FIVE</t>
+        </is>
+      </c>
+      <c r="D122" s="1" t="inlineStr">
+        <is>
+          <t>ACTION</t>
+        </is>
+      </c>
       <c r="E122" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="123">
@@ -2456,11 +2424,11 @@
       <c r="C123" s="1" t="n"/>
       <c r="D123" s="1" t="inlineStr">
         <is>
-          <t>ACTION</t>
+          <t>ACTION - ATTACK</t>
         </is>
       </c>
       <c r="E123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124">
@@ -2469,7 +2437,7 @@
       <c r="C124" s="1" t="n"/>
       <c r="D124" s="1" t="inlineStr">
         <is>
-          <t>ACTION - ATTACK</t>
+          <t>ACTION - ATTACK - LOOTER</t>
         </is>
       </c>
       <c r="E124" t="n">
@@ -2479,37 +2447,37 @@
     <row r="125">
       <c r="A125" s="1" t="n"/>
       <c r="B125" s="1" t="n"/>
-      <c r="C125" s="1" t="inlineStr">
-        <is>
-          <t>FIVE</t>
-        </is>
-      </c>
+      <c r="C125" s="1" t="n"/>
       <c r="D125" s="1" t="inlineStr">
         <is>
-          <t>ACTION</t>
+          <t>TREASURE</t>
         </is>
       </c>
       <c r="E125" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n"/>
       <c r="B126" s="1" t="n"/>
-      <c r="C126" s="1" t="n"/>
+      <c r="C126" s="1" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
       <c r="D126" s="1" t="inlineStr">
         <is>
-          <t>TREASURE</t>
+          <t>ACTION</t>
         </is>
       </c>
       <c r="E126" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>DARK_AGES</t>
+          <t>GUILDS</t>
         </is>
       </c>
       <c r="B127" s="1" t="inlineStr">
@@ -2528,7 +2496,7 @@
         </is>
       </c>
       <c r="E127" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128">
@@ -2536,7 +2504,7 @@
       <c r="B128" s="1" t="n"/>
       <c r="C128" s="1" t="inlineStr">
         <is>
-          <t>THREE</t>
+          <t>FOUR</t>
         </is>
       </c>
       <c r="D128" s="1" t="inlineStr">
@@ -2545,46 +2513,58 @@
         </is>
       </c>
       <c r="E128" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n"/>
       <c r="B129" s="1" t="n"/>
-      <c r="C129" s="1" t="n"/>
+      <c r="C129" s="1" t="inlineStr">
+        <is>
+          <t>FIVE</t>
+        </is>
+      </c>
       <c r="D129" s="1" t="inlineStr">
         <is>
-          <t>ACTION - ATTACK</t>
+          <t>ACTION</t>
         </is>
       </c>
       <c r="E129" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n"/>
       <c r="B130" s="1" t="n"/>
-      <c r="C130" s="1" t="inlineStr">
-        <is>
-          <t>FOUR</t>
-        </is>
-      </c>
-      <c r="D130" s="1" t="inlineStr"/>
+      <c r="C130" s="1" t="n"/>
+      <c r="D130" s="1" t="inlineStr">
+        <is>
+          <t>ACTION - ATTACK</t>
+        </is>
+      </c>
       <c r="E130" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n"/>
-      <c r="B131" s="1" t="n"/>
-      <c r="C131" s="1" t="n"/>
+      <c r="B131" s="1" t="inlineStr">
+        <is>
+          <t>1RC</t>
+        </is>
+      </c>
+      <c r="C131" s="1" t="inlineStr">
+        <is>
+          <t>THREE</t>
+        </is>
+      </c>
       <c r="D131" s="1" t="inlineStr">
         <is>
           <t>ACTION</t>
         </is>
       </c>
       <c r="E131" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
@@ -2593,7 +2573,7 @@
       <c r="C132" s="1" t="n"/>
       <c r="D132" s="1" t="inlineStr">
         <is>
-          <t>ACTION - ATTACK - LOOTER</t>
+          <t>TREASURE</t>
         </is>
       </c>
       <c r="E132" t="n">
@@ -2603,10 +2583,14 @@
     <row r="133">
       <c r="A133" s="1" t="n"/>
       <c r="B133" s="1" t="n"/>
-      <c r="C133" s="1" t="n"/>
+      <c r="C133" s="1" t="inlineStr">
+        <is>
+          <t>FOUR</t>
+        </is>
+      </c>
       <c r="D133" s="1" t="inlineStr">
         <is>
-          <t>ACTION - LOOTER</t>
+          <t>ACTION - ATTACK</t>
         </is>
       </c>
       <c r="E133" t="n">
@@ -2614,11 +2598,19 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="1" t="n"/>
-      <c r="B134" s="1" t="n"/>
+      <c r="A134" s="1" t="inlineStr">
+        <is>
+          <t>ADVENTURES</t>
+        </is>
+      </c>
+      <c r="B134" s="1" t="inlineStr">
+        <is>
+          <t>1ST</t>
+        </is>
+      </c>
       <c r="C134" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>TWO</t>
         </is>
       </c>
       <c r="D134" s="1" t="inlineStr">
@@ -2627,7 +2619,7 @@
         </is>
       </c>
       <c r="E134" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135">
@@ -2636,20 +2628,24 @@
       <c r="C135" s="1" t="n"/>
       <c r="D135" s="1" t="inlineStr">
         <is>
-          <t>ACTION - ATTACK</t>
+          <t>TREASURE</t>
         </is>
       </c>
       <c r="E135" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n"/>
       <c r="B136" s="1" t="n"/>
-      <c r="C136" s="1" t="n"/>
+      <c r="C136" s="1" t="inlineStr">
+        <is>
+          <t>THREE</t>
+        </is>
+      </c>
       <c r="D136" s="1" t="inlineStr">
         <is>
-          <t>ACTION - ATTACK - LOOTER</t>
+          <t>ACTION</t>
         </is>
       </c>
       <c r="E136" t="n">
@@ -2662,11 +2658,11 @@
       <c r="C137" s="1" t="n"/>
       <c r="D137" s="1" t="inlineStr">
         <is>
-          <t>TREASURE</t>
+          <t>ACTION - DURATION</t>
         </is>
       </c>
       <c r="E137" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="138">
@@ -2674,7 +2670,7 @@
       <c r="B138" s="1" t="n"/>
       <c r="C138" s="1" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>FOUR</t>
         </is>
       </c>
       <c r="D138" s="1" t="inlineStr">
@@ -2683,23 +2679,15 @@
         </is>
       </c>
       <c r="E138" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="1" t="inlineStr">
-        <is>
-          <t>ADVENTURES</t>
-        </is>
-      </c>
-      <c r="B139" s="1" t="inlineStr">
-        <is>
-          <t>1ST</t>
-        </is>
-      </c>
+      <c r="A139" s="1" t="n"/>
+      <c r="B139" s="1" t="n"/>
       <c r="C139" s="1" t="inlineStr">
         <is>
-          <t>TWO</t>
+          <t>FIVE</t>
         </is>
       </c>
       <c r="D139" s="1" t="inlineStr">
@@ -2708,7 +2696,7 @@
         </is>
       </c>
       <c r="E139" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="140">
@@ -2717,7 +2705,7 @@
       <c r="C140" s="1" t="n"/>
       <c r="D140" s="1" t="inlineStr">
         <is>
-          <t>TREASURE</t>
+          <t>ACTION - ATTACK</t>
         </is>
       </c>
       <c r="E140" t="n">
@@ -2727,18 +2715,14 @@
     <row r="141">
       <c r="A141" s="1" t="n"/>
       <c r="B141" s="1" t="n"/>
-      <c r="C141" s="1" t="inlineStr">
-        <is>
-          <t>THREE</t>
-        </is>
-      </c>
+      <c r="C141" s="1" t="n"/>
       <c r="D141" s="1" t="inlineStr">
         <is>
-          <t>ACTION</t>
+          <t>ACTION - ATTACK - DURATION</t>
         </is>
       </c>
       <c r="E141" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142">
@@ -2747,28 +2731,24 @@
       <c r="C142" s="1" t="n"/>
       <c r="D142" s="1" t="inlineStr">
         <is>
-          <t>ACTION - DURATION</t>
+          <t>ATTACK - TREASURE</t>
         </is>
       </c>
       <c r="E142" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n"/>
       <c r="B143" s="1" t="n"/>
-      <c r="C143" s="1" t="inlineStr">
-        <is>
-          <t>FOUR</t>
-        </is>
-      </c>
+      <c r="C143" s="1" t="n"/>
       <c r="D143" s="1" t="inlineStr">
         <is>
-          <t>ACTION</t>
+          <t>TREASURE</t>
         </is>
       </c>
       <c r="E143" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
@@ -2776,25 +2756,37 @@
       <c r="B144" s="1" t="n"/>
       <c r="C144" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>OTHER</t>
         </is>
       </c>
       <c r="D144" s="1" t="inlineStr">
         <is>
-          <t>ACTION</t>
+          <t>ACTION - DURATION</t>
         </is>
       </c>
       <c r="E144" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="1" t="n"/>
-      <c r="B145" s="1" t="n"/>
-      <c r="C145" s="1" t="n"/>
+      <c r="A145" s="1" t="inlineStr">
+        <is>
+          <t>CORNUCOPIA_GUILDS</t>
+        </is>
+      </c>
+      <c r="B145" s="1" t="inlineStr">
+        <is>
+          <t>2ND</t>
+        </is>
+      </c>
+      <c r="C145" s="1" t="inlineStr">
+        <is>
+          <t>TWO</t>
+        </is>
+      </c>
       <c r="D145" s="1" t="inlineStr">
         <is>
-          <t>ACTION - ATTACK</t>
+          <t>ACTION</t>
         </is>
       </c>
       <c r="E145" t="n">
@@ -2804,23 +2796,31 @@
     <row r="146">
       <c r="A146" s="1" t="n"/>
       <c r="B146" s="1" t="n"/>
-      <c r="C146" s="1" t="n"/>
+      <c r="C146" s="1" t="inlineStr">
+        <is>
+          <t>THREE</t>
+        </is>
+      </c>
       <c r="D146" s="1" t="inlineStr">
         <is>
-          <t>ACTION - ATTACK - DURATION</t>
+          <t>ACTION</t>
         </is>
       </c>
       <c r="E146" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n"/>
       <c r="B147" s="1" t="n"/>
-      <c r="C147" s="1" t="n"/>
+      <c r="C147" s="1" t="inlineStr">
+        <is>
+          <t>FOUR</t>
+        </is>
+      </c>
       <c r="D147" s="1" t="inlineStr">
         <is>
-          <t>ATTACK - TREASURE</t>
+          <t>ACTION</t>
         </is>
       </c>
       <c r="E147" t="n">
@@ -2830,27 +2830,27 @@
     <row r="148">
       <c r="A148" s="1" t="n"/>
       <c r="B148" s="1" t="n"/>
-      <c r="C148" s="1" t="n"/>
+      <c r="C148" s="1" t="inlineStr">
+        <is>
+          <t>FIVE</t>
+        </is>
+      </c>
       <c r="D148" s="1" t="inlineStr">
         <is>
-          <t>TREASURE</t>
+          <t>ACTION</t>
         </is>
       </c>
       <c r="E148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n"/>
       <c r="B149" s="1" t="n"/>
-      <c r="C149" s="1" t="inlineStr">
-        <is>
-          <t>OTHER</t>
-        </is>
-      </c>
+      <c r="C149" s="1" t="n"/>
       <c r="D149" s="1" t="inlineStr">
         <is>
-          <t>ACTION - DURATION</t>
+          <t>ACTION - ATTACK</t>
         </is>
       </c>
       <c r="E149" t="n">
@@ -4512,12 +4512,13 @@
   </sheetData>
   <mergeCells count="122">
     <mergeCell ref="C231:C239"/>
-    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="A115:A126"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="C225:C226"/>
+    <mergeCell ref="C94:C95"/>
     <mergeCell ref="C162:C165"/>
-    <mergeCell ref="C144:C148"/>
+    <mergeCell ref="C134:C135"/>
     <mergeCell ref="C242:C243"/>
     <mergeCell ref="C87:C89"/>
     <mergeCell ref="C258:C260"/>
@@ -4525,59 +4526,55 @@
     <mergeCell ref="B36:B44"/>
     <mergeCell ref="C251:C254"/>
     <mergeCell ref="C43:C44"/>
-    <mergeCell ref="B139:B149"/>
+    <mergeCell ref="B127:B130"/>
     <mergeCell ref="C60:C63"/>
     <mergeCell ref="B192:B204"/>
     <mergeCell ref="B31:B35"/>
     <mergeCell ref="C69:C70"/>
     <mergeCell ref="C205:C207"/>
-    <mergeCell ref="B98:B100"/>
     <mergeCell ref="C192:C194"/>
-    <mergeCell ref="C111:C112"/>
     <mergeCell ref="C151:C154"/>
     <mergeCell ref="C22:C24"/>
-    <mergeCell ref="B120:B126"/>
     <mergeCell ref="C185:C186"/>
-    <mergeCell ref="C98:C99"/>
     <mergeCell ref="C214:C218"/>
-    <mergeCell ref="A101:A105"/>
-    <mergeCell ref="C122:C124"/>
     <mergeCell ref="C200:C203"/>
-    <mergeCell ref="A139:A149"/>
     <mergeCell ref="C54:C55"/>
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="B71:B76"/>
     <mergeCell ref="B58:B63"/>
     <mergeCell ref="C65:C66"/>
+    <mergeCell ref="A94:A114"/>
     <mergeCell ref="C56:C57"/>
-    <mergeCell ref="C139:C140"/>
+    <mergeCell ref="C148:C149"/>
     <mergeCell ref="A84:A93"/>
     <mergeCell ref="B183:B191"/>
     <mergeCell ref="C248:C250"/>
     <mergeCell ref="A242:A254"/>
-    <mergeCell ref="C134:C137"/>
+    <mergeCell ref="C129:C130"/>
     <mergeCell ref="B150:B161"/>
-    <mergeCell ref="B115:B119"/>
+    <mergeCell ref="B131:B133"/>
+    <mergeCell ref="C131:C132"/>
     <mergeCell ref="B205:B219"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C197:C199"/>
     <mergeCell ref="C40:C42"/>
-    <mergeCell ref="B106:B114"/>
-    <mergeCell ref="B101:B105"/>
     <mergeCell ref="C211:C213"/>
     <mergeCell ref="B242:B254"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="C156:C160"/>
-    <mergeCell ref="C117:C119"/>
-    <mergeCell ref="A106:A126"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="C116:C117"/>
     <mergeCell ref="B220:B241"/>
-    <mergeCell ref="B94:B97"/>
+    <mergeCell ref="C110:C112"/>
     <mergeCell ref="A18:A35"/>
+    <mergeCell ref="C139:C143"/>
     <mergeCell ref="C113:C114"/>
+    <mergeCell ref="B103:B107"/>
     <mergeCell ref="C50:C51"/>
     <mergeCell ref="B255:B261"/>
     <mergeCell ref="C255:C256"/>
     <mergeCell ref="C171:C174"/>
+    <mergeCell ref="C118:C121"/>
     <mergeCell ref="C183:C184"/>
     <mergeCell ref="A192:A204"/>
     <mergeCell ref="B64:B70"/>
@@ -4585,31 +4582,31 @@
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="B91:B93"/>
     <mergeCell ref="C45:C47"/>
+    <mergeCell ref="A127:A133"/>
     <mergeCell ref="C166:C170"/>
     <mergeCell ref="C240:C241"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B94:B102"/>
     <mergeCell ref="C48:C49"/>
     <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C106:C107"/>
+    <mergeCell ref="C122:C125"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="C175:C181"/>
     <mergeCell ref="A255:A261"/>
     <mergeCell ref="A64:A83"/>
     <mergeCell ref="B18:B26"/>
-    <mergeCell ref="A94:A100"/>
+    <mergeCell ref="B134:B144"/>
     <mergeCell ref="B77:B83"/>
+    <mergeCell ref="A145:A149"/>
     <mergeCell ref="C77:C78"/>
     <mergeCell ref="C195:C196"/>
     <mergeCell ref="A36:A57"/>
     <mergeCell ref="B162:B182"/>
     <mergeCell ref="A58:A63"/>
-    <mergeCell ref="C141:C142"/>
-    <mergeCell ref="B127:B138"/>
+    <mergeCell ref="C105:C107"/>
     <mergeCell ref="A183:A191"/>
-    <mergeCell ref="C104:C105"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="C187:C188"/>
-    <mergeCell ref="A127:A138"/>
     <mergeCell ref="A150:A161"/>
     <mergeCell ref="B84:B90"/>
     <mergeCell ref="B14:B17"/>
@@ -4617,21 +4614,24 @@
     <mergeCell ref="C227:C230"/>
     <mergeCell ref="A205:A219"/>
     <mergeCell ref="C25:C26"/>
+    <mergeCell ref="B108:B114"/>
+    <mergeCell ref="C99:C100"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C189:C191"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="B115:B126"/>
     <mergeCell ref="B45:B51"/>
     <mergeCell ref="C67:C68"/>
     <mergeCell ref="C74:C76"/>
     <mergeCell ref="C220:C224"/>
     <mergeCell ref="A162:A182"/>
-    <mergeCell ref="C130:C133"/>
     <mergeCell ref="C72:C73"/>
-    <mergeCell ref="C125:C126"/>
     <mergeCell ref="C96:C97"/>
     <mergeCell ref="A220:A241"/>
+    <mergeCell ref="C136:C137"/>
+    <mergeCell ref="B145:B149"/>
+    <mergeCell ref="B2:B8"/>
     <mergeCell ref="C15:C16"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="C108:C109"/>
     <mergeCell ref="C80:C82"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>